<commit_message>
Adding TC_CALCULATOR_003, removing useless namespaces, updating test plan
</commit_message>
<xml_diff>
--- a/CalculatorTestCases.xlsx
+++ b/CalculatorTestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rock_\OneDrive\Documents\Autodesk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\google_calculator_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E54B5D-37D5-4742-890F-606991F1DCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227D14B9-79BA-45FB-96BA-BA739C1738BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46C4E62A-81F7-4382-B6F4-0CCF39D8DB11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="307">
   <si>
     <t>Project:</t>
   </si>
@@ -103,6 +103,10 @@
     <t>TC_CALCULATOR_006</t>
   </si>
   <si>
+    <t>"1" should be displayed
+in calculator virtual screen.</t>
+  </si>
+  <si>
     <t>TC_CALCULATOR_007</t>
   </si>
   <si>
@@ -114,13 +118,6 @@
   <si>
     <t>Verify that the result of the sum of a 5-digit number plus a 
 4-digit number minus a 2-digit number is correct.</t>
-  </si>
-  <si>
-    <t>"÷"</t>
-  </si>
-  <si>
-    <t>"÷" should be displayed
-in calculator virtual screen.</t>
   </si>
   <si>
     <t>Verify that calculator is displayed after search for "calculator" in search engine page.</t>
@@ -1599,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C3E722-48FC-442D-8B73-FA0B8C94772F}">
   <dimension ref="A1:L204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="B189" sqref="B189"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1666,7 +1663,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
@@ -1698,7 +1695,7 @@
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="14"/>
     </row>
@@ -1707,7 +1704,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
@@ -1723,7 +1720,7 @@
       <c r="A10" s="11"/>
       <c r="B10" s="35"/>
       <c r="D10" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -1738,7 +1735,7 @@
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G11" s="14"/>
     </row>
@@ -1747,19 +1744,19 @@
         <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>29</v>
+        <v>212</v>
+      </c>
+      <c r="E12" s="31">
+        <v>1</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G12" s="32" t="s">
         <v>17</v>
@@ -1770,19 +1767,19 @@
         <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E13" s="11">
         <v>2</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>17</v>
@@ -1792,11 +1789,11 @@
       <c r="A14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G14" s="17"/>
     </row>
@@ -1804,13 +1801,13 @@
       <c r="A15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E15" s="11">
         <v>3</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G15" s="17"/>
     </row>
@@ -1819,11 +1816,11 @@
       <c r="B16" s="15"/>
       <c r="C16" s="8"/>
       <c r="D16" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16" s="18"/>
     </row>
@@ -1832,19 +1829,19 @@
         <v>22</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E17" s="6">
         <v>1</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>17</v>
@@ -1855,11 +1852,11 @@
       <c r="B18" s="9"/>
       <c r="C18" s="11"/>
       <c r="D18" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G18" s="17"/>
     </row>
@@ -1868,13 +1865,13 @@
       <c r="B19" s="9"/>
       <c r="C19" s="11"/>
       <c r="D19" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E19" s="11">
         <v>2</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G19" s="17"/>
     </row>
@@ -1883,11 +1880,11 @@
       <c r="B20" s="9"/>
       <c r="C20" s="11"/>
       <c r="D20" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G20" s="17"/>
     </row>
@@ -1896,13 +1893,13 @@
       <c r="B21" s="9"/>
       <c r="C21" s="11"/>
       <c r="D21" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E21" s="11">
         <v>2</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G21" s="17"/>
     </row>
@@ -1911,11 +1908,11 @@
       <c r="B22" s="15"/>
       <c r="C22" s="8"/>
       <c r="D22" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G22" s="18"/>
     </row>
@@ -1924,19 +1921,19 @@
         <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E23" s="11">
         <v>5</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>17</v>
@@ -1946,11 +1943,11 @@
       <c r="A24" s="10"/>
       <c r="C24" s="11"/>
       <c r="D24" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G24" s="17"/>
     </row>
@@ -1958,13 +1955,13 @@
       <c r="A25" s="10"/>
       <c r="C25" s="11"/>
       <c r="D25" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E25" s="11">
         <v>9</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G25" s="17"/>
     </row>
@@ -1972,11 +1969,11 @@
       <c r="A26" s="10"/>
       <c r="C26" s="11"/>
       <c r="D26" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E26" s="11"/>
       <c r="F26" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G26" s="17"/>
     </row>
@@ -1984,13 +1981,13 @@
       <c r="A27" s="10"/>
       <c r="C27" s="11"/>
       <c r="D27" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E27" s="11">
         <v>7</v>
       </c>
       <c r="F27" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G27" s="17"/>
     </row>
@@ -1998,11 +1995,11 @@
       <c r="A28" s="10"/>
       <c r="C28" s="11"/>
       <c r="D28" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G28" s="17"/>
     </row>
@@ -2010,13 +2007,13 @@
       <c r="A29" s="10"/>
       <c r="C29" s="11"/>
       <c r="D29" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E29" s="11">
         <v>8</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G29" s="17"/>
     </row>
@@ -2024,11 +2021,11 @@
       <c r="A30" s="10"/>
       <c r="C30" s="11"/>
       <c r="D30" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G30" s="17"/>
     </row>
@@ -2036,13 +2033,13 @@
       <c r="A31" s="10"/>
       <c r="C31" s="11"/>
       <c r="D31" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E31" s="11">
         <v>9</v>
       </c>
       <c r="F31" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G31" s="17"/>
     </row>
@@ -2050,11 +2047,11 @@
       <c r="A32" s="10"/>
       <c r="C32" s="11"/>
       <c r="D32" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E32" s="11"/>
       <c r="F32" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G32" s="17"/>
     </row>
@@ -2062,13 +2059,13 @@
       <c r="A33" s="10"/>
       <c r="C33" s="11"/>
       <c r="D33" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E33" s="11">
         <v>3</v>
       </c>
       <c r="F33" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G33" s="17"/>
     </row>
@@ -2076,11 +2073,11 @@
       <c r="A34" s="10"/>
       <c r="C34" s="11"/>
       <c r="D34" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G34" s="17"/>
     </row>
@@ -2088,13 +2085,13 @@
       <c r="A35" s="10"/>
       <c r="C35" s="11"/>
       <c r="D35" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E35" s="11">
         <v>4</v>
       </c>
       <c r="F35" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G35" s="17"/>
     </row>
@@ -2102,11 +2099,11 @@
       <c r="A36" s="10"/>
       <c r="C36" s="11"/>
       <c r="D36" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G36" s="17"/>
     </row>
@@ -2114,13 +2111,13 @@
       <c r="A37" s="10"/>
       <c r="C37" s="11"/>
       <c r="D37" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E37" s="11">
         <v>1</v>
       </c>
       <c r="F37" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G37" s="17"/>
     </row>
@@ -2128,11 +2125,11 @@
       <c r="A38" s="10"/>
       <c r="C38" s="11"/>
       <c r="D38" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G38" s="17"/>
     </row>
@@ -2140,13 +2137,13 @@
       <c r="A39" s="10"/>
       <c r="C39" s="11"/>
       <c r="D39" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E39" s="11">
         <v>6</v>
       </c>
       <c r="F39" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G39" s="17"/>
     </row>
@@ -2155,7 +2152,7 @@
       <c r="B40" s="15"/>
       <c r="C40" s="8"/>
       <c r="D40" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="30" t="s">
@@ -2165,22 +2162,22 @@
     </row>
     <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E41" s="11">
         <v>6</v>
       </c>
       <c r="F41" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>17</v>
@@ -2190,13 +2187,13 @@
       <c r="A42" s="10"/>
       <c r="C42" s="11"/>
       <c r="D42" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E42" s="11">
         <v>2</v>
       </c>
       <c r="F42" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G42" s="17"/>
     </row>
@@ -2204,11 +2201,11 @@
       <c r="A43" s="10"/>
       <c r="C43" s="11"/>
       <c r="D43" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E43" s="11"/>
       <c r="F43" s="29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G43" s="17"/>
     </row>
@@ -2216,13 +2213,13 @@
       <c r="A44" s="10"/>
       <c r="C44" s="11"/>
       <c r="D44" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E44" s="11">
         <v>7</v>
       </c>
       <c r="F44" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G44" s="17"/>
     </row>
@@ -2230,13 +2227,13 @@
       <c r="A45" s="10"/>
       <c r="C45" s="11"/>
       <c r="D45" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E45" s="11">
         <v>5</v>
       </c>
       <c r="F45" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G45" s="17"/>
     </row>
@@ -2244,11 +2241,11 @@
       <c r="A46" s="10"/>
       <c r="C46" s="11"/>
       <c r="D46" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E46" s="11"/>
       <c r="F46" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G46" s="17"/>
     </row>
@@ -2256,13 +2253,13 @@
       <c r="A47" s="10"/>
       <c r="C47" s="11"/>
       <c r="D47" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E47" s="11">
         <v>8</v>
       </c>
       <c r="F47" s="29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G47" s="17"/>
     </row>
@@ -2270,13 +2267,13 @@
       <c r="A48" s="10"/>
       <c r="C48" s="11"/>
       <c r="D48" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E48" s="11">
         <v>4</v>
       </c>
       <c r="F48" s="29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G48" s="17"/>
     </row>
@@ -2285,32 +2282,32 @@
       <c r="B49" s="15"/>
       <c r="C49" s="8"/>
       <c r="D49" s="25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G49" s="18"/>
     </row>
     <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E50" s="11">
         <v>2</v>
       </c>
       <c r="F50" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G50" s="17" t="s">
         <v>17</v>
@@ -2320,11 +2317,11 @@
       <c r="A51" s="10"/>
       <c r="C51" s="11"/>
       <c r="D51" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E51" s="11"/>
       <c r="F51" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G51" s="17"/>
     </row>
@@ -2332,13 +2329,13 @@
       <c r="A52" s="10"/>
       <c r="C52" s="11"/>
       <c r="D52" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E52" s="11">
         <v>3</v>
       </c>
       <c r="F52" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G52" s="17"/>
     </row>
@@ -2347,32 +2344,32 @@
       <c r="B53" s="15"/>
       <c r="C53" s="8"/>
       <c r="D53" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G53" s="18"/>
     </row>
     <row r="54" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E54" s="11">
         <v>5</v>
       </c>
       <c r="F54" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G54" s="17" t="s">
         <v>17</v>
@@ -2382,11 +2379,11 @@
       <c r="A55" s="10"/>
       <c r="C55" s="11"/>
       <c r="D55" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E55" s="11"/>
       <c r="F55" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G55" s="17"/>
     </row>
@@ -2394,13 +2391,13 @@
       <c r="A56" s="10"/>
       <c r="C56" s="11"/>
       <c r="D56" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E56" s="11">
         <v>9</v>
       </c>
       <c r="F56" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G56" s="17"/>
     </row>
@@ -2408,11 +2405,11 @@
       <c r="A57" s="10"/>
       <c r="C57" s="11"/>
       <c r="D57" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E57" s="11"/>
       <c r="F57" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G57" s="17"/>
     </row>
@@ -2420,13 +2417,13 @@
       <c r="A58" s="10"/>
       <c r="C58" s="11"/>
       <c r="D58" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E58" s="11">
         <v>7</v>
       </c>
       <c r="F58" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G58" s="17"/>
     </row>
@@ -2434,11 +2431,11 @@
       <c r="A59" s="10"/>
       <c r="C59" s="11"/>
       <c r="D59" s="12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E59" s="11"/>
       <c r="F59" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G59" s="17"/>
     </row>
@@ -2446,13 +2443,13 @@
       <c r="A60" s="10"/>
       <c r="C60" s="11"/>
       <c r="D60" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E60" s="11">
         <v>8</v>
       </c>
       <c r="F60" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G60" s="17"/>
     </row>
@@ -2460,11 +2457,11 @@
       <c r="A61" s="10"/>
       <c r="C61" s="11"/>
       <c r="D61" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E61" s="11"/>
       <c r="F61" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G61" s="17"/>
     </row>
@@ -2472,13 +2469,13 @@
       <c r="A62" s="10"/>
       <c r="C62" s="11"/>
       <c r="D62" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E62" s="11">
         <v>9</v>
       </c>
       <c r="F62" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G62" s="17"/>
     </row>
@@ -2486,11 +2483,11 @@
       <c r="A63" s="10"/>
       <c r="C63" s="11"/>
       <c r="D63" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E63" s="11"/>
       <c r="F63" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G63" s="17"/>
     </row>
@@ -2498,13 +2495,13 @@
       <c r="A64" s="10"/>
       <c r="C64" s="11"/>
       <c r="D64" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E64" s="11">
         <v>3</v>
       </c>
       <c r="F64" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G64" s="17"/>
     </row>
@@ -2512,11 +2509,11 @@
       <c r="A65" s="10"/>
       <c r="C65" s="11"/>
       <c r="D65" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E65" s="11"/>
       <c r="F65" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G65" s="17"/>
     </row>
@@ -2524,13 +2521,13 @@
       <c r="A66" s="10"/>
       <c r="C66" s="11"/>
       <c r="D66" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E66" s="11">
         <v>4</v>
       </c>
       <c r="F66" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G66" s="17"/>
     </row>
@@ -2538,11 +2535,11 @@
       <c r="A67" s="10"/>
       <c r="C67" s="11"/>
       <c r="D67" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E67" s="11"/>
       <c r="F67" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G67" s="17"/>
     </row>
@@ -2550,13 +2547,13 @@
       <c r="A68" s="10"/>
       <c r="C68" s="11"/>
       <c r="D68" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E68" s="11">
         <v>1</v>
       </c>
       <c r="F68" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G68" s="17"/>
     </row>
@@ -2564,11 +2561,11 @@
       <c r="A69" s="10"/>
       <c r="C69" s="11"/>
       <c r="D69" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E69" s="11"/>
       <c r="F69" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G69" s="17"/>
     </row>
@@ -2576,13 +2573,13 @@
       <c r="A70" s="10"/>
       <c r="C70" s="11"/>
       <c r="D70" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E70" s="11">
         <v>6</v>
       </c>
       <c r="F70" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G70" s="17"/>
     </row>
@@ -2591,32 +2588,32 @@
       <c r="B71" s="15"/>
       <c r="C71" s="8"/>
       <c r="D71" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E71" s="8"/>
       <c r="F71" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G71" s="18"/>
     </row>
     <row r="72" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C72" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E72" s="11">
         <v>2</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G72" s="7" t="s">
         <v>17</v>
@@ -2627,13 +2624,13 @@
       <c r="A73" s="10"/>
       <c r="C73" s="11"/>
       <c r="D73" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E73" s="11">
         <v>3</v>
       </c>
       <c r="F73" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G73" s="13"/>
     </row>
@@ -2641,13 +2638,13 @@
       <c r="A74" s="10"/>
       <c r="C74" s="11"/>
       <c r="D74" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E74" s="11">
         <v>4</v>
       </c>
       <c r="F74" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G74" s="13"/>
     </row>
@@ -2655,11 +2652,11 @@
       <c r="A75" s="10"/>
       <c r="C75" s="11"/>
       <c r="D75" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E75" s="11"/>
       <c r="F75" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G75" s="13"/>
     </row>
@@ -2667,13 +2664,13 @@
       <c r="A76" s="10"/>
       <c r="C76" s="11"/>
       <c r="D76" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E76" s="11">
         <v>5</v>
       </c>
       <c r="F76" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G76" s="13"/>
     </row>
@@ -2681,13 +2678,13 @@
       <c r="A77" s="10"/>
       <c r="C77" s="11"/>
       <c r="D77" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E77" s="11">
         <v>6</v>
       </c>
       <c r="F77" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G77" s="13"/>
     </row>
@@ -2695,13 +2692,13 @@
       <c r="A78" s="10"/>
       <c r="C78" s="11"/>
       <c r="D78" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E78" s="11">
         <v>9</v>
       </c>
       <c r="F78" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G78" s="13"/>
     </row>
@@ -2709,11 +2706,11 @@
       <c r="A79" s="10"/>
       <c r="C79" s="11"/>
       <c r="D79" s="12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E79" s="11"/>
       <c r="F79" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G79" s="13"/>
     </row>
@@ -2721,13 +2718,13 @@
       <c r="A80" s="10"/>
       <c r="C80" s="11"/>
       <c r="D80" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E80" s="11">
         <v>2</v>
       </c>
       <c r="F80" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G80" s="13"/>
     </row>
@@ -2735,13 +2732,13 @@
       <c r="A81" s="10"/>
       <c r="C81" s="11"/>
       <c r="D81" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E81" s="11">
         <v>6</v>
       </c>
       <c r="F81" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G81" s="13"/>
     </row>
@@ -2749,13 +2746,13 @@
       <c r="A82" s="10"/>
       <c r="C82" s="11"/>
       <c r="D82" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E82" s="11">
         <v>1</v>
       </c>
       <c r="F82" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G82" s="13"/>
     </row>
@@ -2763,11 +2760,11 @@
       <c r="A83" s="10"/>
       <c r="C83" s="11"/>
       <c r="D83" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E83" s="11"/>
       <c r="F83" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G83" s="13"/>
     </row>
@@ -2775,13 +2772,13 @@
       <c r="A84" s="10"/>
       <c r="C84" s="11"/>
       <c r="D84" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E84" s="11">
         <v>4</v>
       </c>
       <c r="F84" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G84" s="13"/>
     </row>
@@ -2789,13 +2786,13 @@
       <c r="A85" s="10"/>
       <c r="C85" s="11"/>
       <c r="D85" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E85" s="11">
         <v>5</v>
       </c>
       <c r="F85" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G85" s="13"/>
     </row>
@@ -2803,13 +2800,13 @@
       <c r="A86" s="10"/>
       <c r="C86" s="11"/>
       <c r="D86" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E86" s="11">
         <v>8</v>
       </c>
       <c r="F86" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G86" s="13"/>
     </row>
@@ -2818,32 +2815,32 @@
       <c r="B87" s="15"/>
       <c r="C87" s="8"/>
       <c r="D87" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E87" s="8"/>
       <c r="F87" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G87" s="18"/>
     </row>
     <row r="88" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B88" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E88" s="24">
         <v>9</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G88" s="16" t="s">
         <v>17</v>
@@ -2854,13 +2851,13 @@
       <c r="B89" s="9"/>
       <c r="C89" s="11"/>
       <c r="D89" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E89" s="11">
         <v>9</v>
       </c>
       <c r="F89" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G89" s="17"/>
     </row>
@@ -2869,13 +2866,13 @@
       <c r="B90" s="9"/>
       <c r="C90" s="11"/>
       <c r="D90" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E90" s="11">
         <v>5</v>
       </c>
       <c r="F90" s="29" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G90" s="17"/>
     </row>
@@ -2884,13 +2881,13 @@
       <c r="B91" s="9"/>
       <c r="C91" s="11"/>
       <c r="D91" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E91" s="11">
         <v>3</v>
       </c>
       <c r="F91" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G91" s="17"/>
     </row>
@@ -2899,13 +2896,13 @@
       <c r="B92" s="9"/>
       <c r="C92" s="11"/>
       <c r="D92" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E92" s="11">
         <v>7</v>
       </c>
       <c r="F92" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G92" s="17"/>
     </row>
@@ -2914,11 +2911,11 @@
       <c r="B93" s="9"/>
       <c r="C93" s="11"/>
       <c r="D93" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E93" s="11"/>
       <c r="F93" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G93" s="17"/>
     </row>
@@ -2927,13 +2924,13 @@
       <c r="B94" s="9"/>
       <c r="C94" s="11"/>
       <c r="D94" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E94" s="11">
         <v>3</v>
       </c>
       <c r="F94" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G94" s="17"/>
     </row>
@@ -2942,13 +2939,13 @@
       <c r="B95" s="9"/>
       <c r="C95" s="11"/>
       <c r="D95" s="12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E95" s="11">
         <v>5</v>
       </c>
       <c r="F95" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G95" s="17"/>
     </row>
@@ -2957,13 +2954,13 @@
       <c r="B96" s="9"/>
       <c r="C96" s="11"/>
       <c r="D96" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E96" s="11">
         <v>8</v>
       </c>
       <c r="F96" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G96" s="17"/>
     </row>
@@ -2972,13 +2969,13 @@
       <c r="B97" s="9"/>
       <c r="C97" s="11"/>
       <c r="D97" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E97" s="11">
         <v>6</v>
       </c>
       <c r="F97" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G97" s="17"/>
     </row>
@@ -2987,11 +2984,11 @@
       <c r="B98" s="9"/>
       <c r="C98" s="11"/>
       <c r="D98" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E98" s="11"/>
       <c r="F98" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G98" s="17"/>
     </row>
@@ -3000,13 +2997,13 @@
       <c r="B99" s="9"/>
       <c r="C99" s="11"/>
       <c r="D99" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E99" s="11">
         <v>7</v>
       </c>
       <c r="F99" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G99" s="17"/>
     </row>
@@ -3015,13 +3012,13 @@
       <c r="B100" s="9"/>
       <c r="C100" s="11"/>
       <c r="D100" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E100" s="11">
         <v>4</v>
       </c>
       <c r="F100" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G100" s="17"/>
     </row>
@@ -3030,32 +3027,32 @@
       <c r="B101" s="15"/>
       <c r="C101" s="8"/>
       <c r="D101" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E101" s="8"/>
       <c r="F101" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G101" s="18"/>
     </row>
     <row r="102" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A102" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B102" s="41" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D102" s="40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E102" s="39">
         <v>8</v>
       </c>
       <c r="F102" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G102" s="7" t="s">
         <v>17</v>
@@ -3066,13 +3063,13 @@
       <c r="B103" s="10"/>
       <c r="C103" s="10"/>
       <c r="D103" s="39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E103" s="39">
         <v>1</v>
       </c>
       <c r="F103" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G103" s="13"/>
     </row>
@@ -3081,13 +3078,13 @@
       <c r="B104" s="10"/>
       <c r="C104" s="10"/>
       <c r="D104" s="39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E104" s="39">
         <v>9</v>
       </c>
       <c r="F104" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G104" s="13"/>
     </row>
@@ -3096,10 +3093,10 @@
       <c r="B105" s="10"/>
       <c r="C105" s="10"/>
       <c r="D105" s="39" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F105" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G105" s="13"/>
     </row>
@@ -3108,13 +3105,13 @@
       <c r="B106" s="10"/>
       <c r="C106" s="10"/>
       <c r="D106" s="39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E106">
         <v>6</v>
       </c>
       <c r="F106" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G106" s="13"/>
     </row>
@@ -3123,13 +3120,13 @@
       <c r="B107" s="10"/>
       <c r="C107" s="10"/>
       <c r="D107" s="39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E107">
         <v>5</v>
       </c>
       <c r="F107" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G107" s="13"/>
     </row>
@@ -3138,13 +3135,13 @@
       <c r="B108" s="10"/>
       <c r="C108" s="10"/>
       <c r="D108" s="39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E108">
         <v>2</v>
       </c>
       <c r="F108" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G108" s="13"/>
     </row>
@@ -3153,10 +3150,10 @@
       <c r="B109" s="10"/>
       <c r="C109" s="10"/>
       <c r="D109" s="39" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F109" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G109" s="13"/>
     </row>
@@ -3165,13 +3162,13 @@
       <c r="B110" s="10"/>
       <c r="C110" s="10"/>
       <c r="D110" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E110">
         <v>4</v>
       </c>
       <c r="F110" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G110" s="13"/>
     </row>
@@ -3180,10 +3177,10 @@
       <c r="B111" s="10"/>
       <c r="C111" s="10"/>
       <c r="D111" s="39" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F111" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G111" s="13"/>
     </row>
@@ -3192,13 +3189,13 @@
       <c r="B112" s="10"/>
       <c r="C112" s="10"/>
       <c r="D112" s="39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E112">
         <v>9</v>
       </c>
       <c r="F112" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G112" s="13"/>
     </row>
@@ -3207,10 +3204,10 @@
       <c r="B113" s="10"/>
       <c r="C113" s="10"/>
       <c r="D113" s="39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F113" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G113" s="13"/>
     </row>
@@ -3219,13 +3216,13 @@
       <c r="B114" s="10"/>
       <c r="C114" s="10"/>
       <c r="D114" s="39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E114">
         <v>8</v>
       </c>
       <c r="F114" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G114" s="13"/>
     </row>
@@ -3234,10 +3231,10 @@
       <c r="B115" s="10"/>
       <c r="C115" s="10"/>
       <c r="D115" s="39" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F115" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G115" s="13"/>
     </row>
@@ -3246,13 +3243,13 @@
       <c r="B116" s="10"/>
       <c r="C116" s="10"/>
       <c r="D116" s="39" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E116" s="9">
         <v>3</v>
       </c>
       <c r="F116" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G116" s="13"/>
     </row>
@@ -3261,32 +3258,32 @@
       <c r="B117" s="23"/>
       <c r="C117" s="23"/>
       <c r="D117" s="42" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E117" s="15"/>
       <c r="F117" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G117" s="14"/>
     </row>
     <row r="118" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B118" s="41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C118" s="22" t="s">
         <v>19</v>
       </c>
       <c r="D118" s="40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E118" s="19">
         <v>8</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G118" s="7" t="s">
         <v>17</v>
@@ -3297,11 +3294,11 @@
       <c r="B119" s="10"/>
       <c r="C119" s="10"/>
       <c r="D119" s="39" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E119" s="9"/>
       <c r="F119" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G119" s="13"/>
     </row>
@@ -3310,13 +3307,13 @@
       <c r="B120" s="10"/>
       <c r="C120" s="10"/>
       <c r="D120" s="39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E120" s="9">
         <v>4</v>
       </c>
       <c r="F120" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G120" s="13"/>
     </row>
@@ -3325,13 +3322,13 @@
       <c r="B121" s="10"/>
       <c r="C121" s="10"/>
       <c r="D121" s="39" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E121" s="9">
         <v>0</v>
       </c>
       <c r="F121" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G121" s="13"/>
     </row>
@@ -3340,11 +3337,11 @@
       <c r="B122" s="10"/>
       <c r="C122" s="10"/>
       <c r="D122" s="39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E122" s="9"/>
       <c r="F122" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G122" s="13"/>
     </row>
@@ -3353,13 +3350,13 @@
       <c r="B123" s="10"/>
       <c r="C123" s="10"/>
       <c r="D123" s="39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E123" s="9">
         <v>3</v>
       </c>
       <c r="F123" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G123" s="13"/>
     </row>
@@ -3368,13 +3365,13 @@
       <c r="B124" s="10"/>
       <c r="C124" s="10"/>
       <c r="D124" s="39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E124" s="9">
         <v>8</v>
       </c>
       <c r="F124" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G124" s="13"/>
     </row>
@@ -3383,32 +3380,32 @@
       <c r="B125" s="23"/>
       <c r="C125" s="23"/>
       <c r="D125" s="42" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E125" s="15"/>
       <c r="F125" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G125" s="14"/>
     </row>
     <row r="126" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B126" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="B126" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D126" s="40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E126" s="12">
         <v>7</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G126" s="7" t="s">
         <v>17</v>
@@ -3419,10 +3416,10 @@
       <c r="B127" s="11"/>
       <c r="C127" s="11"/>
       <c r="D127" s="39" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F127" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G127" s="13"/>
     </row>
@@ -3431,13 +3428,13 @@
       <c r="B128" s="11"/>
       <c r="C128" s="11"/>
       <c r="D128" s="39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E128">
         <v>8</v>
       </c>
       <c r="F128" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G128" s="13"/>
     </row>
@@ -3446,13 +3443,13 @@
       <c r="B129" s="11"/>
       <c r="C129" s="11"/>
       <c r="D129" s="39" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E129">
         <v>6</v>
       </c>
       <c r="F129" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G129" s="13"/>
     </row>
@@ -3461,10 +3458,10 @@
       <c r="B130" s="11"/>
       <c r="C130" s="11"/>
       <c r="D130" s="39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F130" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G130" s="13"/>
     </row>
@@ -3473,13 +3470,13 @@
       <c r="B131" s="11"/>
       <c r="C131" s="11"/>
       <c r="D131" s="39" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E131">
         <v>5</v>
       </c>
       <c r="F131" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G131" s="13"/>
     </row>
@@ -3488,10 +3485,10 @@
       <c r="B132" s="11"/>
       <c r="C132" s="11"/>
       <c r="D132" s="39" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F132" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G132" s="13"/>
     </row>
@@ -3500,13 +3497,13 @@
       <c r="B133" s="11"/>
       <c r="C133" s="11"/>
       <c r="D133" s="39" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E133">
         <v>4</v>
       </c>
       <c r="F133" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G133" s="13"/>
     </row>
@@ -3515,13 +3512,13 @@
       <c r="B134" s="11"/>
       <c r="C134" s="11"/>
       <c r="D134" s="39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E134">
         <v>1</v>
       </c>
       <c r="F134" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G134" s="13"/>
     </row>
@@ -3530,32 +3527,32 @@
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
       <c r="D135" s="42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E135" s="15"/>
       <c r="F135" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G135" s="14"/>
     </row>
     <row r="136" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B136" s="41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C136" s="22" t="s">
         <v>19</v>
       </c>
       <c r="D136" s="40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E136" s="12">
         <v>7</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G136" s="7" t="s">
         <v>17</v>
@@ -3566,13 +3563,13 @@
       <c r="B137" s="10"/>
       <c r="C137" s="10"/>
       <c r="D137" s="39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E137" s="12">
         <v>9</v>
       </c>
       <c r="F137" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G137" s="13"/>
     </row>
@@ -3581,13 +3578,13 @@
       <c r="B138" s="10"/>
       <c r="C138" s="10"/>
       <c r="D138" s="39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E138" s="12">
         <v>6</v>
       </c>
       <c r="F138" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G138" s="13"/>
     </row>
@@ -3596,10 +3593,10 @@
       <c r="B139" s="10"/>
       <c r="C139" s="10"/>
       <c r="D139" s="39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F139" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G139" s="13"/>
     </row>
@@ -3608,13 +3605,13 @@
       <c r="B140" s="10"/>
       <c r="C140" s="10"/>
       <c r="D140" s="39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E140">
         <v>1</v>
       </c>
       <c r="F140" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G140" s="13"/>
     </row>
@@ -3623,13 +3620,13 @@
       <c r="B141" s="10"/>
       <c r="C141" s="10"/>
       <c r="D141" s="39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E141">
         <v>2</v>
       </c>
       <c r="F141" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G141" s="13"/>
     </row>
@@ -3638,13 +3635,13 @@
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
       <c r="D142" s="39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E142">
         <v>5</v>
       </c>
       <c r="F142" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G142" s="13"/>
     </row>
@@ -3653,32 +3650,32 @@
       <c r="B143" s="23"/>
       <c r="C143" s="23"/>
       <c r="D143" s="42" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E143" s="15"/>
       <c r="F143" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G143" s="14"/>
     </row>
     <row r="144" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C144" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D144" s="40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E144" s="19">
         <v>5</v>
       </c>
       <c r="F144" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G144" s="7" t="s">
         <v>17</v>
@@ -3689,11 +3686,11 @@
       <c r="B145" s="11"/>
       <c r="C145" s="11"/>
       <c r="D145" s="39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E145" s="9"/>
       <c r="F145" s="29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G145" s="13"/>
     </row>
@@ -3702,13 +3699,13 @@
       <c r="B146" s="11"/>
       <c r="C146" s="11"/>
       <c r="D146" s="39" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E146" s="9">
         <v>0</v>
       </c>
       <c r="F146" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G146" s="13"/>
     </row>
@@ -3717,32 +3714,32 @@
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
       <c r="D147" s="42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E147" s="15"/>
       <c r="F147" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G147" s="14"/>
     </row>
     <row r="148" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A148" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D148" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E148" s="6">
         <v>5</v>
       </c>
       <c r="F148" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G148" s="7" t="s">
         <v>17</v>
@@ -3753,13 +3750,13 @@
       <c r="B149" s="11"/>
       <c r="C149" s="11"/>
       <c r="D149" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E149" s="11">
         <v>2</v>
       </c>
       <c r="F149" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G149" s="13"/>
     </row>
@@ -3768,11 +3765,11 @@
       <c r="B150" s="11"/>
       <c r="C150" s="11"/>
       <c r="D150" s="33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E150" s="11"/>
       <c r="F150" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G150" s="13"/>
     </row>
@@ -3781,13 +3778,13 @@
       <c r="B151" s="11"/>
       <c r="C151" s="11"/>
       <c r="D151" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E151" s="11">
         <v>3</v>
       </c>
       <c r="F151" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G151" s="13"/>
     </row>
@@ -3796,13 +3793,13 @@
       <c r="B152" s="11"/>
       <c r="C152" s="11"/>
       <c r="D152" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E152" s="11">
         <v>3</v>
       </c>
       <c r="F152" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G152" s="13"/>
     </row>
@@ -3811,11 +3808,11 @@
       <c r="B153" s="11"/>
       <c r="C153" s="11"/>
       <c r="D153" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E153" s="11"/>
       <c r="F153" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G153" s="13"/>
     </row>
@@ -3824,13 +3821,13 @@
       <c r="B154" s="11"/>
       <c r="C154" s="11"/>
       <c r="D154" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E154" s="11">
         <v>9</v>
       </c>
       <c r="F154" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G154" s="13"/>
     </row>
@@ -3839,11 +3836,11 @@
       <c r="B155" s="11"/>
       <c r="C155" s="11"/>
       <c r="D155" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E155" s="11"/>
       <c r="F155" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G155" s="13"/>
     </row>
@@ -3852,13 +3849,13 @@
       <c r="B156" s="11"/>
       <c r="C156" s="11"/>
       <c r="D156" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E156" s="11">
         <v>1</v>
       </c>
       <c r="F156" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G156" s="13"/>
     </row>
@@ -3867,11 +3864,11 @@
       <c r="B157" s="11"/>
       <c r="C157" s="11"/>
       <c r="D157" s="33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E157" s="11"/>
       <c r="F157" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G157" s="13"/>
     </row>
@@ -3880,13 +3877,13 @@
       <c r="B158" s="11"/>
       <c r="C158" s="11"/>
       <c r="D158" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E158" s="11">
         <v>6</v>
       </c>
       <c r="F158" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G158" s="13"/>
     </row>
@@ -3895,32 +3892,32 @@
       <c r="B159" s="8"/>
       <c r="C159" s="8"/>
       <c r="D159" s="43" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E159" s="8"/>
       <c r="F159" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G159" s="14"/>
     </row>
     <row r="160" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" s="26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C160" s="22" t="s">
         <v>19</v>
       </c>
       <c r="D160" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E160" s="6">
         <v>3</v>
       </c>
       <c r="F160" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G160" s="7" t="s">
         <v>17</v>
@@ -3931,13 +3928,13 @@
       <c r="B161" s="11"/>
       <c r="C161" s="9"/>
       <c r="D161" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E161" s="11">
         <v>4</v>
       </c>
       <c r="F161" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G161" s="13"/>
     </row>
@@ -3946,11 +3943,11 @@
       <c r="B162" s="11"/>
       <c r="C162" s="9"/>
       <c r="D162" s="33" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E162" s="11"/>
       <c r="F162" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G162" s="13"/>
     </row>
@@ -3959,13 +3956,13 @@
       <c r="B163" s="11"/>
       <c r="C163" s="9"/>
       <c r="D163" s="33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E163" s="11">
         <v>7</v>
       </c>
       <c r="F163" s="29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G163" s="13"/>
     </row>
@@ -3974,13 +3971,13 @@
       <c r="B164" s="11"/>
       <c r="C164" s="9"/>
       <c r="D164" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E164" s="11">
         <v>5</v>
       </c>
       <c r="F164" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G164" s="13"/>
     </row>
@@ -3989,11 +3986,11 @@
       <c r="B165" s="11"/>
       <c r="C165" s="9"/>
       <c r="D165" s="33" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E165" s="11"/>
       <c r="F165" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G165" s="13"/>
     </row>
@@ -4002,13 +3999,13 @@
       <c r="B166" s="11"/>
       <c r="C166" s="9"/>
       <c r="D166" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E166" s="11">
         <v>6</v>
       </c>
       <c r="F166" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G166" s="13"/>
     </row>
@@ -4017,11 +4014,11 @@
       <c r="B167" s="11"/>
       <c r="C167" s="9"/>
       <c r="D167" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E167" s="11"/>
       <c r="F167" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G167" s="13"/>
     </row>
@@ -4030,13 +4027,13 @@
       <c r="B168" s="11"/>
       <c r="C168" s="9"/>
       <c r="D168" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E168" s="11">
         <v>2</v>
       </c>
       <c r="F168" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G168" s="13"/>
     </row>
@@ -4045,13 +4042,13 @@
       <c r="B169" s="11"/>
       <c r="C169" s="9"/>
       <c r="D169" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E169" s="11">
         <v>9</v>
       </c>
       <c r="F169" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G169" s="13"/>
     </row>
@@ -4060,13 +4057,13 @@
       <c r="B170" s="11"/>
       <c r="C170" s="9"/>
       <c r="D170" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E170" s="11">
         <v>4</v>
       </c>
       <c r="F170" s="29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G170" s="13"/>
     </row>
@@ -4075,32 +4072,32 @@
       <c r="B171" s="8"/>
       <c r="C171" s="15"/>
       <c r="D171" s="43" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E171" s="8"/>
       <c r="F171" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G171" s="14"/>
     </row>
     <row r="172" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B172" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="B172" s="5" t="s">
-        <v>192</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D172" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E172" s="24">
         <v>7</v>
       </c>
       <c r="F172" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G172" s="7" t="s">
         <v>17</v>
@@ -4111,11 +4108,11 @@
       <c r="B173" s="11"/>
       <c r="C173" s="11"/>
       <c r="D173" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E173" s="11"/>
       <c r="F173" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G173" s="13"/>
     </row>
@@ -4124,13 +4121,13 @@
       <c r="B174" s="11"/>
       <c r="C174" s="11"/>
       <c r="D174" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E174" s="11">
         <v>2</v>
       </c>
       <c r="F174" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G174" s="13"/>
     </row>
@@ -4139,11 +4136,11 @@
       <c r="B175" s="11"/>
       <c r="C175" s="11"/>
       <c r="D175" s="33" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E175" s="11"/>
       <c r="F175" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G175" s="13"/>
     </row>
@@ -4152,13 +4149,13 @@
       <c r="B176" s="11"/>
       <c r="C176" s="11"/>
       <c r="D176" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E176" s="11">
         <v>5</v>
       </c>
       <c r="F176" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G176" s="13"/>
     </row>
@@ -4167,11 +4164,11 @@
       <c r="B177" s="11"/>
       <c r="C177" s="11"/>
       <c r="D177" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E177" s="11"/>
       <c r="F177" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G177" s="13"/>
     </row>
@@ -4180,13 +4177,13 @@
       <c r="B178" s="11"/>
       <c r="C178" s="11"/>
       <c r="D178" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E178" s="11">
         <v>4</v>
       </c>
       <c r="F178" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G178" s="13"/>
     </row>
@@ -4195,13 +4192,13 @@
       <c r="B179" s="11"/>
       <c r="C179" s="11"/>
       <c r="D179" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E179" s="11">
         <v>6</v>
       </c>
       <c r="F179" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G179" s="13"/>
     </row>
@@ -4210,11 +4207,11 @@
       <c r="B180" s="11"/>
       <c r="C180" s="11"/>
       <c r="D180" s="33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E180" s="11"/>
       <c r="F180" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G180" s="13"/>
     </row>
@@ -4223,13 +4220,13 @@
       <c r="B181" s="11"/>
       <c r="C181" s="11"/>
       <c r="D181" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E181" s="11">
         <v>8</v>
       </c>
       <c r="F181" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G181" s="13"/>
     </row>
@@ -4238,11 +4235,11 @@
       <c r="B182" s="11"/>
       <c r="C182" s="11"/>
       <c r="D182" s="33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E182" s="11"/>
       <c r="F182" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G182" s="13"/>
     </row>
@@ -4251,13 +4248,13 @@
       <c r="B183" s="11"/>
       <c r="C183" s="11"/>
       <c r="D183" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E183" s="11">
         <v>2</v>
       </c>
       <c r="F183" s="29" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G183" s="13"/>
     </row>
@@ -4266,30 +4263,30 @@
       <c r="B184" s="8"/>
       <c r="C184" s="8"/>
       <c r="D184" s="43" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E184" s="8"/>
       <c r="F184" s="30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G184" s="14"/>
     </row>
     <row r="185" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A185" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B185" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="B185" s="5" t="s">
-        <v>212</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D185" s="34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E185" s="6"/>
       <c r="F185" s="29" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G185" s="7" t="s">
         <v>17</v>
@@ -4300,11 +4297,11 @@
       <c r="B186" s="11"/>
       <c r="C186" s="11"/>
       <c r="D186" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E186" s="11"/>
       <c r="F186" s="29" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G186" s="13"/>
     </row>
@@ -4313,13 +4310,13 @@
       <c r="B187" s="11"/>
       <c r="C187" s="11"/>
       <c r="D187" s="33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E187" s="11">
         <v>9</v>
       </c>
       <c r="F187" s="29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G187" s="13"/>
     </row>
@@ -4328,32 +4325,32 @@
       <c r="B188" s="8"/>
       <c r="C188" s="8"/>
       <c r="D188" s="43" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E188" s="8"/>
       <c r="F188" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G188" s="14"/>
     </row>
     <row r="189" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A189" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C189" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D189" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E189" s="6">
         <v>2</v>
       </c>
       <c r="F189" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G189" s="7" t="s">
         <v>17</v>
@@ -4364,11 +4361,11 @@
       <c r="B190" s="11"/>
       <c r="C190" s="11"/>
       <c r="D190" s="33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E190" s="11"/>
       <c r="F190" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G190" s="13"/>
     </row>
@@ -4377,13 +4374,13 @@
       <c r="B191" s="11"/>
       <c r="C191" s="11"/>
       <c r="D191" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E191" s="11">
         <v>3</v>
       </c>
       <c r="F191" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G191" s="13"/>
     </row>
@@ -4392,11 +4389,11 @@
       <c r="B192" s="11"/>
       <c r="C192" s="11"/>
       <c r="D192" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E192" s="11"/>
       <c r="F192" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G192" s="13"/>
     </row>
@@ -4405,11 +4402,11 @@
       <c r="B193" s="11"/>
       <c r="C193" s="11"/>
       <c r="D193" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E193" s="11"/>
       <c r="F193" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G193" s="13"/>
     </row>
@@ -4418,13 +4415,13 @@
       <c r="B194" s="11"/>
       <c r="C194" s="11"/>
       <c r="D194" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E194" s="11">
         <v>6</v>
       </c>
       <c r="F194" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G194" s="13"/>
     </row>
@@ -4433,11 +4430,11 @@
       <c r="B195" s="11"/>
       <c r="C195" s="11"/>
       <c r="D195" s="33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E195" s="11"/>
       <c r="F195" s="29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G195" s="13"/>
     </row>
@@ -4446,13 +4443,13 @@
       <c r="B196" s="11"/>
       <c r="C196" s="11"/>
       <c r="D196" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E196" s="11">
         <v>2</v>
       </c>
       <c r="F196" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G196" s="13"/>
     </row>
@@ -4461,11 +4458,11 @@
       <c r="B197" s="11"/>
       <c r="C197" s="11"/>
       <c r="D197" s="33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E197" s="11"/>
       <c r="F197" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G197" s="13"/>
     </row>
@@ -4474,13 +4471,13 @@
       <c r="B198" s="11"/>
       <c r="C198" s="11"/>
       <c r="D198" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E198" s="11">
         <v>5</v>
       </c>
       <c r="F198" s="29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G198" s="13"/>
     </row>
@@ -4489,32 +4486,32 @@
       <c r="B199" s="8"/>
       <c r="C199" s="8"/>
       <c r="D199" s="43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E199" s="8"/>
       <c r="F199" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G199" s="14"/>
     </row>
     <row r="200" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A200" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D200" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E200" s="6">
         <v>7</v>
       </c>
       <c r="F200" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G200" s="7" t="s">
         <v>17</v>
@@ -4525,11 +4522,11 @@
       <c r="B201" s="11"/>
       <c r="C201" s="11"/>
       <c r="D201" s="33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E201" s="11"/>
       <c r="F201" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G201" s="13"/>
     </row>
@@ -4538,13 +4535,13 @@
       <c r="B202" s="11"/>
       <c r="C202" s="11"/>
       <c r="D202" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E202" s="11">
         <v>2</v>
       </c>
       <c r="F202" s="29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G202" s="13"/>
     </row>
@@ -4553,11 +4550,11 @@
       <c r="B203" s="11"/>
       <c r="C203" s="11"/>
       <c r="D203" s="33" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E203" s="11"/>
       <c r="F203" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G203" s="13"/>
     </row>
@@ -4566,11 +4563,11 @@
       <c r="B204" s="8"/>
       <c r="C204" s="8"/>
       <c r="D204" s="43" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E204" s="8"/>
       <c r="F204" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G204" s="14"/>
     </row>

</xml_diff>

<commit_message>
Adding From TC_CALCULATOR_010 to TC_CALCULATOR_022
</commit_message>
<xml_diff>
--- a/CalculatorTestCases.xlsx
+++ b/CalculatorTestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\google_calculator_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227D14B9-79BA-45FB-96BA-BA739C1738BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEE34DC-73F2-452F-8A2E-02757C2C4312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46C4E62A-81F7-4382-B6F4-0CCF39D8DB11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="307">
   <si>
     <t>Project:</t>
   </si>
@@ -1596,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C3E722-48FC-442D-8B73-FA0B8C94772F}">
   <dimension ref="A1:L204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="D199" sqref="D199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4486,7 +4486,7 @@
       <c r="B199" s="8"/>
       <c r="C199" s="8"/>
       <c r="D199" s="43" t="s">
-        <v>261</v>
+        <v>215</v>
       </c>
       <c r="E199" s="8"/>
       <c r="F199" s="30" t="s">

</xml_diff>